<commit_message>
tax treatment of child care costs corrected and tested (#9)
</commit_message>
<xml_diff>
--- a/src/analysis/tax_transfer_funcs/test_tax_transfers/test_data/test_dfs_zve.xlsx
+++ b/src/analysis/tax_transfer_funcs/test_tax_transfers/test_data/test_dfs_zve.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6500ACB2-FCA8-4850-9CF3-657957F62E5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="zve" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>tu_id</t>
   </si>
@@ -120,11 +128,14 @@
   <si>
     <t>ineducation</t>
   </si>
+  <si>
+    <t>m_childcare</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -178,7 +189,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -194,7 +205,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -269,6 +280,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -304,6 +332,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -479,21 +524,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AM30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM27" sqref="AM27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="14" width="13.7109375" customWidth="1"/>
-    <col min="15" max="15" width="16.7109375" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" style="1"/>
+    <col min="13" max="15" width="13.7109375" customWidth="1"/>
+    <col min="16" max="16" width="16.7109375" customWidth="1"/>
+    <col min="25" max="25" width="9.140625" style="1"/>
+    <col min="34" max="34" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -537,70 +583,73 @@
         <v>19</v>
       </c>
       <c r="O1" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>4</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>26</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>3</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>5</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>17</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>24</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>B2</f>
         <v>1</v>
@@ -624,11 +673,11 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <f t="shared" ref="H2:H19" si="0">W2+(65-U2)</f>
+        <f t="shared" ref="H2:H19" si="0">X2+(65-V2)</f>
         <v>2043</v>
       </c>
       <c r="I2">
-        <f>(N2=FALSE)*40+(N2=TRUE)</f>
+        <f t="shared" ref="I2:I30" si="1">(N2=FALSE)*40+(N2=TRUE)</f>
         <v>40</v>
       </c>
       <c r="J2" t="b">
@@ -664,54 +713,57 @@
       <c r="S2">
         <v>0</v>
       </c>
-      <c r="T2" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>40</v>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
         <v>2018</v>
       </c>
-      <c r="X2" s="2">
-        <f t="shared" ref="X2:X13" si="1">MAX(AD2-AC2-36,0)</f>
-        <v>0</v>
-      </c>
       <c r="Y2" s="2">
-        <f t="shared" ref="Y2:Y14" si="2">X2-AE2</f>
-        <v>0</v>
-      </c>
-      <c r="Z2" s="1">
-        <f>X2+MAX(F2*12-801-36,0)</f>
+        <f t="shared" ref="Y2:Y13" si="2">MAX(AE2-AD2-36,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z2" s="2">
+        <f t="shared" ref="Z2:Z14" si="3">Y2-AF2</f>
+        <v>0</v>
+      </c>
+      <c r="AA2" s="1">
+        <f>Y2+MAX(F2*12-801-36,0)</f>
         <v>363</v>
       </c>
-      <c r="AA2" s="1">
-        <f>MAX(Z2-AE3,0)</f>
+      <c r="AB2" s="1">
+        <f>MAX(AA2-AF3,0)</f>
         <v>363</v>
       </c>
-      <c r="AC2">
-        <f t="shared" ref="AC2:AC12" si="3">INT(((0.6+(0.02*(W2-2005)))*(2*12*P2))-(12*P2))+AF2</f>
-        <v>0</v>
-      </c>
       <c r="AD2">
-        <f t="shared" ref="AD2:AD7" si="4">(12*E2+(12*D2 - 1000)*(D2&gt;450))</f>
+        <f t="shared" ref="AD2:AD12" si="4">INT(((0.6+(0.02*(X2-2005)))*(2*12*Q2))-(12*Q2))+AG2</f>
         <v>0</v>
       </c>
       <c r="AE2">
+        <f t="shared" ref="AE2:AE7" si="5">(12*E2+(12*D2 - 1000)*(D2&gt;450))</f>
         <v>0</v>
       </c>
       <c r="AF2">
-        <f t="shared" ref="AF2:AF27" si="5">INT(MAX(12 *(0.96*R2+S2), MIN(12 *(0.96*R2+S2+Q2),  1900)  ))</f>
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <f t="shared" ref="AG2:AG27" si="6">INT(MAX(12 *(0.96*S2+T2), MIN(12 *(0.96*S2+T2+R2),  1900)  ))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A13" si="6">B3</f>
+        <f t="shared" ref="A3:A13" si="7">B3</f>
         <v>2</v>
       </c>
       <c r="B3">
@@ -737,7 +789,7 @@
         <v>2043</v>
       </c>
       <c r="I3">
-        <f>(N3=FALSE)*40+(N3=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J3" t="b">
@@ -762,69 +814,72 @@
         <v>0</v>
       </c>
       <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
         <f>0.1*$D3</f>
         <v>60</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <f>0.02*D3</f>
         <v>12</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <f>0.08*D3</f>
         <v>48</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <f>0.015*D3</f>
         <v>9</v>
       </c>
-      <c r="T3" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>40</v>
+      <c r="U3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
         <v>2018</v>
-      </c>
-      <c r="X3" s="2">
-        <f t="shared" si="1"/>
-        <v>4842</v>
       </c>
       <c r="Y3" s="2">
         <f t="shared" si="2"/>
         <v>4842</v>
       </c>
-      <c r="Z3" s="1">
-        <f>X3+MAX(F3*12-801,0)</f>
+      <c r="Z3" s="2">
+        <f t="shared" si="3"/>
+        <v>4842</v>
+      </c>
+      <c r="AA3" s="1">
+        <f>Y3+MAX(F3*12-801,0)</f>
         <v>5241</v>
       </c>
-      <c r="AA3" s="1">
-        <f t="shared" ref="AA3:AA14" si="7">MAX(Z3-AE3,0)</f>
+      <c r="AB3" s="1">
+        <f t="shared" ref="AB3:AB14" si="8">MAX(AA3-AF3,0)</f>
         <v>5241</v>
-      </c>
-      <c r="AC3">
-        <f t="shared" si="3"/>
-        <v>1322</v>
       </c>
       <c r="AD3">
         <f t="shared" si="4"/>
+        <v>1322</v>
+      </c>
+      <c r="AE3">
+        <f t="shared" si="5"/>
         <v>6200</v>
       </c>
-      <c r="AE3">
-        <v>0</v>
-      </c>
       <c r="AF3">
-        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <f t="shared" si="6"/>
         <v>804</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="B4">
@@ -850,7 +905,7 @@
         <v>2043</v>
       </c>
       <c r="I4">
-        <f>(N4=FALSE)*40+(N4=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J4" t="b">
@@ -875,69 +930,72 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <f t="shared" ref="P4:P13" si="8">0.1*D4</f>
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ref="Q4:Q13" si="9">0.1*D4</f>
         <v>90</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <f>0.02*D4</f>
         <v>18</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <f>0.08*D4</f>
         <v>72</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <f>0.015*D4</f>
         <v>13.5</v>
       </c>
-      <c r="T4" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>40</v>
+      <c r="U4" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
         <v>2018</v>
-      </c>
-      <c r="X4" s="2">
-        <f t="shared" si="1"/>
-        <v>7780</v>
       </c>
       <c r="Y4" s="2">
         <f t="shared" si="2"/>
         <v>7780</v>
       </c>
-      <c r="Z4" s="1">
-        <f>X4+MAX(F4*12-801,0)</f>
+      <c r="Z4" s="2">
+        <f t="shared" si="3"/>
+        <v>7780</v>
+      </c>
+      <c r="AA4" s="1">
+        <f>Y4+MAX(F4*12-801,0)</f>
         <v>8179</v>
       </c>
-      <c r="AA4" s="1">
-        <f t="shared" si="7"/>
+      <c r="AB4" s="1">
+        <f t="shared" si="8"/>
         <v>8179</v>
-      </c>
-      <c r="AC4">
-        <f t="shared" si="3"/>
-        <v>1984</v>
       </c>
       <c r="AD4">
         <f t="shared" si="4"/>
+        <v>1984</v>
+      </c>
+      <c r="AE4">
+        <f t="shared" si="5"/>
         <v>9800</v>
       </c>
-      <c r="AE4">
-        <v>0</v>
-      </c>
       <c r="AF4">
-        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <f t="shared" si="6"/>
         <v>1207</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="B5">
@@ -963,7 +1021,7 @@
         <v>2043</v>
       </c>
       <c r="I5">
-        <f>(N5=FALSE)*40+(N5=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J5" t="b">
@@ -988,69 +1046,72 @@
         <v>0</v>
       </c>
       <c r="P5">
-        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="9"/>
         <v>120</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <f>0.02*D5</f>
         <v>24</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <f>0.08*D5</f>
         <v>96</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <f>0.015*D5</f>
         <v>18</v>
       </c>
-      <c r="T5" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>40</v>
+      <c r="U5" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="V5">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
         <v>2018</v>
-      </c>
-      <c r="X5" s="2">
-        <f t="shared" si="1"/>
-        <v>10719</v>
       </c>
       <c r="Y5" s="2">
         <f t="shared" si="2"/>
         <v>10719</v>
       </c>
-      <c r="Z5" s="1">
-        <f>X5+MAX(F5*12-801,0)</f>
+      <c r="Z5" s="2">
+        <f t="shared" si="3"/>
+        <v>10719</v>
+      </c>
+      <c r="AA5" s="1">
+        <f>Y5+MAX(F5*12-801,0)</f>
         <v>11118</v>
       </c>
-      <c r="AA5" s="1">
-        <f t="shared" si="7"/>
+      <c r="AB5" s="1">
+        <f t="shared" si="8"/>
         <v>11118</v>
-      </c>
-      <c r="AC5">
-        <f t="shared" si="3"/>
-        <v>2645</v>
       </c>
       <c r="AD5">
         <f t="shared" si="4"/>
+        <v>2645</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" si="5"/>
         <v>13400</v>
       </c>
-      <c r="AE5">
-        <v>0</v>
-      </c>
       <c r="AF5">
-        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <f t="shared" si="6"/>
         <v>1609</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="B6">
@@ -1076,7 +1137,7 @@
         <v>2043</v>
       </c>
       <c r="I6">
-        <f>(N6=FALSE)*40+(N6=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J6" t="b">
@@ -1101,69 +1162,72 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="9"/>
         <v>150</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <f>0.02*D6</f>
         <v>30</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <f>0.08*D6</f>
         <v>120</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <f>0.015*D6</f>
         <v>22.5</v>
       </c>
-      <c r="T6" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>40</v>
+      <c r="U6" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="V6">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
         <v>2018</v>
-      </c>
-      <c r="X6" s="2">
-        <f t="shared" si="1"/>
-        <v>13768</v>
       </c>
       <c r="Y6" s="2">
         <f t="shared" si="2"/>
         <v>13768</v>
       </c>
-      <c r="Z6" s="1">
-        <f>X6+MAX(F6*12-801,0)</f>
+      <c r="Z6" s="2">
+        <f t="shared" si="3"/>
+        <v>13768</v>
+      </c>
+      <c r="AA6" s="1">
+        <f>Y6+MAX(F6*12-801,0)</f>
         <v>14167</v>
       </c>
-      <c r="AA6" s="1">
-        <f t="shared" si="7"/>
+      <c r="AB6" s="1">
+        <f t="shared" si="8"/>
         <v>14167</v>
-      </c>
-      <c r="AC6">
-        <f t="shared" si="3"/>
-        <v>3196</v>
       </c>
       <c r="AD6">
         <f t="shared" si="4"/>
+        <v>3196</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" si="5"/>
         <v>17000</v>
       </c>
-      <c r="AE6">
-        <v>0</v>
-      </c>
       <c r="AF6">
-        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <f t="shared" si="6"/>
         <v>1900</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="B7">
@@ -1189,7 +1253,7 @@
         <v>2043</v>
       </c>
       <c r="I7">
-        <f>(N7=FALSE)*40+(N7=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J7" t="b">
@@ -1214,69 +1278,72 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="9"/>
         <v>500</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <f>0.02*D7</f>
         <v>100</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <f>0.08*D7</f>
         <v>400</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <f>0.015*D7</f>
         <v>75</v>
       </c>
-      <c r="T7" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>40</v>
+      <c r="U7" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
         <v>2018</v>
-      </c>
-      <c r="X7" s="2">
-        <f t="shared" si="1"/>
-        <v>49136</v>
       </c>
       <c r="Y7" s="2">
         <f t="shared" si="2"/>
         <v>49136</v>
       </c>
-      <c r="Z7" s="1">
-        <f>X7+MAX(F7*12-801,0)</f>
+      <c r="Z7" s="2">
+        <f t="shared" si="3"/>
+        <v>49136</v>
+      </c>
+      <c r="AA7" s="1">
+        <f>Y7+MAX(F7*12-801,0)</f>
         <v>49535</v>
       </c>
-      <c r="AA7" s="1">
-        <f t="shared" si="7"/>
+      <c r="AB7" s="1">
+        <f t="shared" si="8"/>
         <v>49535</v>
-      </c>
-      <c r="AC7">
-        <f t="shared" si="3"/>
-        <v>9828</v>
       </c>
       <c r="AD7">
         <f t="shared" si="4"/>
+        <v>9828</v>
+      </c>
+      <c r="AE7">
+        <f t="shared" si="5"/>
         <v>59000</v>
       </c>
-      <c r="AE7">
-        <v>0</v>
-      </c>
       <c r="AF7">
-        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <f t="shared" si="6"/>
         <v>5508</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
       <c r="B8">
@@ -1302,7 +1369,7 @@
         <v>2035</v>
       </c>
       <c r="I8">
-        <f>(N8=FALSE)*40+(N8=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J8" t="b">
@@ -1338,54 +1405,57 @@
       <c r="S8">
         <v>0</v>
       </c>
-      <c r="T8" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>40</v>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="V8">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
         <v>2010</v>
-      </c>
-      <c r="X8" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
       <c r="Y8" s="2">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Z8" s="1">
-        <f>X8+MAX(F8*12-801-36,0)</f>
+      <c r="Z8" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA8" s="1">
+        <f>Y8+MAX(F8*12-801-36,0)</f>
         <v>363</v>
       </c>
-      <c r="AA8" s="1">
+      <c r="AB8" s="1">
+        <f t="shared" si="8"/>
+        <v>363</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <f t="shared" ref="AE8:AE13" si="10">(12*E8+(12*D8 - 920)*(D8&gt;450))</f>
+        <v>0</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A9">
         <f t="shared" si="7"/>
-        <v>363</v>
-      </c>
-      <c r="AC8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AD8">
-        <f t="shared" ref="AD8:AD13" si="9">(12*E8+(12*D8 - 920)*(D8&gt;450))</f>
-        <v>0</v>
-      </c>
-      <c r="AE8">
-        <v>0</v>
-      </c>
-      <c r="AF8">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="B9">
@@ -1411,7 +1481,7 @@
         <v>2035</v>
       </c>
       <c r="I9">
-        <f>(N9=FALSE)*40+(N9=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J9" t="b">
@@ -1436,69 +1506,72 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <f>0.02*D9</f>
         <v>12</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <f>0.08*D9</f>
         <v>48</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <f>0.015*D9</f>
         <v>9</v>
       </c>
-      <c r="T9" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U9">
-        <v>40</v>
+      <c r="U9" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="V9">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
         <v>2010</v>
-      </c>
-      <c r="X9" s="2">
-        <f t="shared" si="1"/>
-        <v>5152</v>
       </c>
       <c r="Y9" s="2">
         <f t="shared" si="2"/>
         <v>5152</v>
       </c>
-      <c r="Z9" s="1">
-        <f t="shared" ref="Z9:Z14" si="10">X9+MAX(F9*12-801,0)</f>
+      <c r="Z9" s="2">
+        <f t="shared" si="3"/>
+        <v>5152</v>
+      </c>
+      <c r="AA9" s="1">
+        <f t="shared" ref="AA9:AA14" si="11">Y9+MAX(F9*12-801,0)</f>
         <v>5551</v>
       </c>
-      <c r="AA9" s="1">
+      <c r="AB9" s="1">
+        <f t="shared" si="8"/>
+        <v>5551</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="4"/>
+        <v>1092</v>
+      </c>
+      <c r="AE9">
+        <f t="shared" si="10"/>
+        <v>6280</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <f t="shared" si="6"/>
+        <v>804</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A10">
         <f t="shared" si="7"/>
-        <v>5551</v>
-      </c>
-      <c r="AC9">
-        <f t="shared" si="3"/>
-        <v>1092</v>
-      </c>
-      <c r="AD9">
-        <f t="shared" si="9"/>
-        <v>6280</v>
-      </c>
-      <c r="AE9">
-        <v>0</v>
-      </c>
-      <c r="AF9">
-        <f t="shared" si="5"/>
-        <v>804</v>
-      </c>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="B10">
@@ -1524,7 +1597,7 @@
         <v>2035</v>
       </c>
       <c r="I10">
-        <f>(N10=FALSE)*40+(N10=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J10" t="b">
@@ -1549,69 +1622,72 @@
         <v>0</v>
       </c>
       <c r="P10">
-        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="9"/>
         <v>90</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <f>0.02*D10</f>
         <v>18</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <f>0.08*D10</f>
         <v>72</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <f>0.015*D10</f>
         <v>13.5</v>
       </c>
-      <c r="T10" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>40</v>
+      <c r="U10" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="V10">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
         <v>2010</v>
-      </c>
-      <c r="X10" s="2">
-        <f t="shared" si="1"/>
-        <v>8205</v>
       </c>
       <c r="Y10" s="2">
         <f t="shared" si="2"/>
         <v>8205</v>
       </c>
-      <c r="Z10" s="1">
+      <c r="Z10" s="2">
+        <f t="shared" si="3"/>
+        <v>8205</v>
+      </c>
+      <c r="AA10" s="1">
+        <f t="shared" si="11"/>
+        <v>8604</v>
+      </c>
+      <c r="AB10" s="1">
+        <f t="shared" si="8"/>
+        <v>8604</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="4"/>
+        <v>1639</v>
+      </c>
+      <c r="AE10">
         <f t="shared" si="10"/>
-        <v>8604</v>
-      </c>
-      <c r="AA10" s="1">
+        <v>9880</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <f t="shared" si="6"/>
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A11">
         <f t="shared" si="7"/>
-        <v>8604</v>
-      </c>
-      <c r="AC10">
-        <f t="shared" si="3"/>
-        <v>1639</v>
-      </c>
-      <c r="AD10">
-        <f t="shared" si="9"/>
-        <v>9880</v>
-      </c>
-      <c r="AE10">
-        <v>0</v>
-      </c>
-      <c r="AF10">
-        <f t="shared" si="5"/>
-        <v>1207</v>
-      </c>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="B11">
@@ -1637,7 +1713,7 @@
         <v>2035</v>
       </c>
       <c r="I11">
-        <f>(N11=FALSE)*40+(N11=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J11" t="b">
@@ -1662,69 +1738,72 @@
         <v>0</v>
       </c>
       <c r="P11">
-        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="9"/>
         <v>120</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <f>0.02*D11</f>
         <v>24</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <f>0.08*D11</f>
         <v>96</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <f>0.015*D11</f>
         <v>18</v>
       </c>
-      <c r="T11" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>40</v>
+      <c r="U11" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="V11">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
         <v>2010</v>
-      </c>
-      <c r="X11" s="2">
-        <f t="shared" si="1"/>
-        <v>11259</v>
       </c>
       <c r="Y11" s="2">
         <f t="shared" si="2"/>
         <v>11259</v>
       </c>
-      <c r="Z11" s="1">
+      <c r="Z11" s="2">
+        <f t="shared" si="3"/>
+        <v>11259</v>
+      </c>
+      <c r="AA11" s="1">
+        <f t="shared" si="11"/>
+        <v>11658</v>
+      </c>
+      <c r="AB11" s="1">
+        <f t="shared" si="8"/>
+        <v>11658</v>
+      </c>
+      <c r="AD11">
+        <f t="shared" si="4"/>
+        <v>2185</v>
+      </c>
+      <c r="AE11">
         <f t="shared" si="10"/>
-        <v>11658</v>
-      </c>
-      <c r="AA11" s="1">
+        <v>13480</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <f t="shared" si="6"/>
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A12">
         <f t="shared" si="7"/>
-        <v>11658</v>
-      </c>
-      <c r="AC11">
-        <f t="shared" si="3"/>
-        <v>2185</v>
-      </c>
-      <c r="AD11">
-        <f t="shared" si="9"/>
-        <v>13480</v>
-      </c>
-      <c r="AE11">
-        <v>0</v>
-      </c>
-      <c r="AF11">
-        <f t="shared" si="5"/>
-        <v>1609</v>
-      </c>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="B12">
@@ -1750,7 +1829,7 @@
         <v>2035</v>
       </c>
       <c r="I12">
-        <f>(N12=FALSE)*40+(N12=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J12" t="b">
@@ -1775,69 +1854,72 @@
         <v>0</v>
       </c>
       <c r="P12">
-        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="9"/>
         <v>150</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <f>0.02*D12</f>
         <v>30</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <f>0.08*D12</f>
         <v>120</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <f>0.015*D12</f>
         <v>22.5</v>
       </c>
-      <c r="T12" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>40</v>
+      <c r="U12" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="V12">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
         <v>2010</v>
-      </c>
-      <c r="X12" s="2">
-        <f t="shared" si="1"/>
-        <v>14424</v>
       </c>
       <c r="Y12" s="2">
         <f t="shared" si="2"/>
         <v>14424</v>
       </c>
-      <c r="Z12" s="1">
+      <c r="Z12" s="2">
+        <f t="shared" si="3"/>
+        <v>14424</v>
+      </c>
+      <c r="AA12" s="1">
+        <f t="shared" si="11"/>
+        <v>14823</v>
+      </c>
+      <c r="AB12" s="1">
+        <f t="shared" si="8"/>
+        <v>14823</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="4"/>
+        <v>2620</v>
+      </c>
+      <c r="AE12">
         <f t="shared" si="10"/>
-        <v>14823</v>
-      </c>
-      <c r="AA12" s="1">
+        <v>17080</v>
+      </c>
+      <c r="AF12">
+        <v>0</v>
+      </c>
+      <c r="AG12">
+        <f t="shared" si="6"/>
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A13">
         <f t="shared" si="7"/>
-        <v>14823</v>
-      </c>
-      <c r="AC12">
-        <f t="shared" si="3"/>
-        <v>2620</v>
-      </c>
-      <c r="AD12">
-        <f t="shared" si="9"/>
-        <v>17080</v>
-      </c>
-      <c r="AE12">
-        <v>0</v>
-      </c>
-      <c r="AF12">
-        <f t="shared" si="5"/>
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="B13">
@@ -1863,7 +1945,7 @@
         <v>2035</v>
       </c>
       <c r="I13">
-        <f>(N13=FALSE)*40+(N13=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J13" t="b">
@@ -1888,67 +1970,70 @@
         <v>0</v>
       </c>
       <c r="P13">
-        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="9"/>
         <v>800</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <f>0.02*D13</f>
         <v>160</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <f>0.08*D13</f>
         <v>640</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <f>0.015*D13</f>
         <v>120</v>
       </c>
-      <c r="T13" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <v>40</v>
+      <c r="U13" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="V13">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
         <v>2010</v>
-      </c>
-      <c r="X13" s="2">
-        <f t="shared" si="1"/>
-        <v>83606</v>
       </c>
       <c r="Y13" s="2">
         <f t="shared" si="2"/>
         <v>83606</v>
       </c>
-      <c r="Z13" s="1">
+      <c r="Z13" s="2">
+        <f t="shared" si="3"/>
+        <v>83606</v>
+      </c>
+      <c r="AA13" s="1">
+        <f t="shared" si="11"/>
+        <v>84005</v>
+      </c>
+      <c r="AB13" s="1">
+        <f t="shared" si="8"/>
+        <v>84005</v>
+      </c>
+      <c r="AD13">
+        <f>INT(((0.6+(0.02*(X13-2005)))*(12*2*0.0995*5500))-(12*0.0995*5500))+AG13</f>
+        <v>11438</v>
+      </c>
+      <c r="AE13">
         <f t="shared" si="10"/>
-        <v>84005</v>
-      </c>
-      <c r="AA13" s="1">
-        <f t="shared" si="7"/>
-        <v>84005</v>
-      </c>
-      <c r="AC13">
-        <f>INT(((0.6+(0.02*(W13-2005)))*(12*2*0.0995*5500))-(12*0.0995*5500))+AF13</f>
-        <v>11438</v>
-      </c>
-      <c r="AD13">
-        <f t="shared" si="9"/>
         <v>95080</v>
       </c>
-      <c r="AE13">
-        <v>0</v>
-      </c>
       <c r="AF13">
-        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG13">
+        <f t="shared" si="6"/>
         <v>8812</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>21</v>
       </c>
@@ -1975,7 +2060,7 @@
         <v>2037</v>
       </c>
       <c r="I14">
-        <f>(N14=FALSE)*40+(N14=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J14" t="b">
@@ -2000,68 +2085,71 @@
         <v>0</v>
       </c>
       <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
         <f>0.1*$D14</f>
         <v>200</v>
       </c>
-      <c r="Q14">
-        <f t="shared" ref="Q14:Q19" si="11">0.02*D14</f>
-        <v>40</v>
-      </c>
       <c r="R14">
-        <f t="shared" ref="R14:R19" si="12">0.08*D14</f>
+        <f t="shared" ref="R14:R19" si="12">0.02*D14</f>
+        <v>40</v>
+      </c>
+      <c r="S14">
+        <f t="shared" ref="S14:S19" si="13">0.08*D14</f>
         <v>160</v>
       </c>
-      <c r="S14">
-        <f t="shared" ref="S14:S19" si="13">0.015*D14</f>
+      <c r="T14">
+        <f t="shared" ref="T14:T19" si="14">0.015*D14</f>
         <v>30</v>
       </c>
-      <c r="T14" t="b">
+      <c r="U14" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="U14">
-        <v>40</v>
-      </c>
       <c r="V14">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14">
         <v>2012</v>
       </c>
-      <c r="X14" s="2">
-        <f>MAX(AD14-AC14-36-1308,0)</f>
+      <c r="Y14" s="2">
+        <f>MAX(AE14-AD14-36-1308,0)</f>
         <v>18301</v>
       </c>
-      <c r="Y14" s="2">
-        <f t="shared" si="2"/>
+      <c r="Z14" s="2">
+        <f t="shared" si="3"/>
         <v>14797</v>
       </c>
-      <c r="Z14" s="1">
-        <f t="shared" si="10"/>
+      <c r="AA14" s="1">
+        <f t="shared" si="11"/>
         <v>18700</v>
       </c>
-      <c r="AA14" s="1">
-        <f t="shared" si="7"/>
+      <c r="AB14" s="1">
+        <f t="shared" si="8"/>
         <v>15196</v>
       </c>
-      <c r="AC14">
-        <f t="shared" ref="AC14:AC27" si="14">INT(((0.6+(0.02*(W14-2005)))*(2*12*P14))-(12*P14))+AF14</f>
+      <c r="AD14">
+        <f t="shared" ref="AD14:AD27" si="15">INT(((0.6+(0.02*(X14-2005)))*(2*12*Q14))-(12*Q14))+AG14</f>
         <v>3355</v>
       </c>
-      <c r="AD14">
+      <c r="AE14">
         <f>(12*E14+(12*D14 - 1000)*(D14&gt;450))</f>
         <v>23000</v>
       </c>
-      <c r="AE14">
+      <c r="AF14">
         <f>0.5*7008</f>
         <v>3504</v>
       </c>
-      <c r="AF14">
-        <f t="shared" si="5"/>
+      <c r="AG14">
+        <f t="shared" si="6"/>
         <v>2203</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>21</v>
       </c>
@@ -2088,7 +2176,7 @@
         <v>2072</v>
       </c>
       <c r="I15">
-        <f>(N15=FALSE)*40+(N15=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J15" t="b">
@@ -2113,11 +2201,10 @@
         <v>0</v>
       </c>
       <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
         <f>0.1*$D15</f>
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R15">
@@ -2128,40 +2215,44 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="T15" t="b">
+      <c r="T15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="U15" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>5</v>
       </c>
-      <c r="V15">
-        <v>1</v>
-      </c>
       <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15">
         <v>2012</v>
       </c>
-      <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
-      <c r="Z15" s="1"/>
+      <c r="Z15" s="2"/>
       <c r="AA15" s="1"/>
-      <c r="AC15">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
+      <c r="AB15" s="1"/>
       <c r="AD15">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE15">
         <f>(12*E15+(12*D15 - 1000)*(D15&gt;450))</f>
         <v>0</v>
       </c>
-      <c r="AE15">
-        <v>0</v>
-      </c>
       <c r="AF15">
-        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>22</v>
       </c>
@@ -2188,7 +2279,7 @@
         <v>2034</v>
       </c>
       <c r="I16">
-        <f>(N16=FALSE)*40+(N16=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J16" t="b">
@@ -2213,68 +2304,71 @@
         <v>0</v>
       </c>
       <c r="P16">
-        <f t="shared" ref="P16:P19" si="15">0.1*D16</f>
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" ref="Q16:Q19" si="16">0.1*D16</f>
         <v>300</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="11"/>
-        <v>60</v>
       </c>
       <c r="R16">
         <f t="shared" si="12"/>
-        <v>240</v>
+        <v>60</v>
       </c>
       <c r="S16">
         <f t="shared" si="13"/>
+        <v>240</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="14"/>
         <v>45</v>
       </c>
-      <c r="T16" t="b">
+      <c r="U16" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="U16">
-        <v>40</v>
-      </c>
       <c r="V16">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
         <v>2009</v>
       </c>
-      <c r="X16" s="2">
-        <f>MAX(AD16-AC16-36-1308,0)</f>
+      <c r="Y16" s="2">
+        <f>MAX(AE16-AD16-36-1308,0)</f>
         <v>29136</v>
       </c>
-      <c r="Y16" s="2">
-        <f>X16-AE16</f>
+      <c r="Z16" s="2">
+        <f>Y16-AF16</f>
         <v>26124</v>
       </c>
-      <c r="Z16" s="1">
-        <f>X16+MAX(F16*12-801,0)</f>
+      <c r="AA16" s="1">
+        <f>Y16+MAX(F16*12-801,0)</f>
         <v>29535</v>
       </c>
-      <c r="AA16" s="1">
-        <f>MAX(Z16-AE16,0)</f>
+      <c r="AB16" s="1">
+        <f>MAX(AA16-AF16,0)</f>
         <v>26523</v>
       </c>
-      <c r="AC16">
-        <f t="shared" si="14"/>
+      <c r="AD16">
+        <f t="shared" si="15"/>
         <v>4600</v>
       </c>
-      <c r="AD16">
+      <c r="AE16">
         <f>(12*E16+(12*D16 - 920)*(D16&gt;450))</f>
         <v>35080</v>
       </c>
-      <c r="AE16">
+      <c r="AF16">
         <f>0.5*6024</f>
         <v>3012</v>
       </c>
-      <c r="AF16">
-        <f t="shared" si="5"/>
+      <c r="AG16">
+        <f t="shared" si="6"/>
         <v>3304</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>22</v>
       </c>
@@ -2301,7 +2395,7 @@
         <v>2069</v>
       </c>
       <c r="I17">
-        <f>(N17=FALSE)*40+(N17=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J17" t="b">
@@ -2326,11 +2420,10 @@
         <v>0</v>
       </c>
       <c r="P17">
-        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R17">
@@ -2341,40 +2434,44 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="T17" t="b">
+      <c r="T17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="U17" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>5</v>
       </c>
-      <c r="V17">
-        <v>1</v>
-      </c>
       <c r="W17">
+        <v>1</v>
+      </c>
+      <c r="X17">
         <v>2009</v>
       </c>
-      <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
-      <c r="Z17" s="1"/>
+      <c r="Z17" s="2"/>
       <c r="AA17" s="1"/>
-      <c r="AC17">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
+      <c r="AB17" s="1"/>
       <c r="AD17">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="AE17">
         <f>(12*E17+(12*D17 - 1000)*(D17&gt;450))</f>
         <v>0</v>
       </c>
-      <c r="AE17">
-        <v>0</v>
-      </c>
       <c r="AF17">
-        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG17">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>23</v>
       </c>
@@ -2401,7 +2498,7 @@
         <v>2030</v>
       </c>
       <c r="I18">
-        <f>(N18=FALSE)*40+(N18=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J18" t="b">
@@ -2426,68 +2523,71 @@
         <v>0</v>
       </c>
       <c r="P18">
-        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="16"/>
         <v>200</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="11"/>
-        <v>40</v>
       </c>
       <c r="R18">
         <f t="shared" si="12"/>
-        <v>160</v>
+        <v>40</v>
       </c>
       <c r="S18">
         <f t="shared" si="13"/>
+        <v>160</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="14"/>
         <v>30</v>
       </c>
-      <c r="T18" t="b">
+      <c r="U18" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="U18">
-        <v>40</v>
-      </c>
       <c r="V18">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="W18">
+        <v>1</v>
+      </c>
+      <c r="X18">
         <v>2005</v>
       </c>
-      <c r="X18" s="2">
-        <f>MAX(AD18-AC18-36-1308,0)</f>
+      <c r="Y18" s="2">
+        <f>MAX(AE18-AD18-36-1308,0)</f>
         <v>29632</v>
       </c>
-      <c r="Y18" s="2">
-        <f>X18-AE18</f>
+      <c r="Z18" s="2">
+        <f>Y18-AF18</f>
         <v>26728</v>
       </c>
-      <c r="Z18" s="1">
-        <f>X18+MAX(F18*12-1370-51,0)</f>
+      <c r="AA18" s="1">
+        <f>Y18+MAX(F18*12-1370-51,0)</f>
         <v>40211</v>
       </c>
-      <c r="AA18" s="1">
-        <f>MAX(Z18-AE18,0)</f>
+      <c r="AB18" s="1">
+        <f>MAX(AA18-AF18,0)</f>
         <v>37307</v>
       </c>
-      <c r="AC18">
-        <f t="shared" si="14"/>
+      <c r="AD18">
+        <f t="shared" si="15"/>
         <v>2683</v>
       </c>
-      <c r="AD18">
+      <c r="AE18">
         <f>(12*E18+((12*D18)-920)*(D18&gt;450)+MAX((12*F18)-51-1370,0))</f>
         <v>33659</v>
       </c>
-      <c r="AE18">
+      <c r="AF18">
         <f>5808/2</f>
         <v>2904</v>
       </c>
-      <c r="AF18">
-        <f t="shared" si="5"/>
+      <c r="AG18">
+        <f t="shared" si="6"/>
         <v>2203</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>23</v>
       </c>
@@ -2514,7 +2614,7 @@
         <v>2065</v>
       </c>
       <c r="I19">
-        <f>(N19=FALSE)*40+(N19=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J19" t="b">
@@ -2539,11 +2639,10 @@
         <v>0</v>
       </c>
       <c r="P19">
-        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R19">
@@ -2554,40 +2653,44 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="T19" t="b">
+      <c r="T19">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="U19" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <v>5</v>
       </c>
-      <c r="V19">
-        <v>1</v>
-      </c>
       <c r="W19">
+        <v>1</v>
+      </c>
+      <c r="X19">
         <v>2005</v>
       </c>
-      <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
-      <c r="Z19" s="1"/>
+      <c r="Z19" s="2"/>
       <c r="AA19" s="1"/>
-      <c r="AC19">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
+      <c r="AB19" s="1"/>
       <c r="AD19">
-        <f t="shared" ref="AD19:AD30" si="16">(12*E19+(12*D19 - 1000)*(D19&gt;450))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AE19">
+        <f t="shared" ref="AE19:AE30" si="17">(12*E19+(12*D19 - 1000)*(D19&gt;450))</f>
         <v>0</v>
       </c>
       <c r="AF19">
-        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG19">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>31</v>
       </c>
@@ -2610,11 +2713,11 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <f>W20+(65-U20)</f>
+        <f>X20+(65-V20)</f>
         <v>2053</v>
       </c>
       <c r="I20">
-        <f>(N20=FALSE)*40+(N20=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J20" t="b">
@@ -2639,67 +2742,70 @@
         <v>0</v>
       </c>
       <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
         <f>0.1*$D20</f>
         <v>200</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <f>0.02*D20</f>
         <v>40</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <f>0.08*D20</f>
         <v>160</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <f>0.015*D20</f>
         <v>30</v>
       </c>
-      <c r="T20" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U20">
+      <c r="U20" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="V20">
         <v>30</v>
       </c>
-      <c r="V20">
-        <v>0</v>
-      </c>
       <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
         <v>2018</v>
       </c>
-      <c r="X20" s="2">
-        <f>MAX(AD20-AC20-36,0)</f>
+      <c r="Y20" s="2">
+        <f>MAX(AE20-AD20-36,0)</f>
         <v>19033</v>
       </c>
-      <c r="Y20" s="2">
-        <f>X20-AE20</f>
+      <c r="Z20" s="2">
+        <f>Y20-AF20</f>
         <v>19033</v>
       </c>
-      <c r="Z20" s="1">
-        <f>X20+MAX(F20*12-801,0)</f>
+      <c r="AA20" s="1">
+        <f>Y20+MAX(F20*12-801,0)</f>
         <v>19033</v>
       </c>
-      <c r="AA20" s="1">
-        <f>MAX(Z20-AE20,0)</f>
+      <c r="AB20" s="1">
+        <f>MAX(AA20-AF20,0)</f>
         <v>19033</v>
       </c>
-      <c r="AC20">
-        <f t="shared" si="14"/>
+      <c r="AD20">
+        <f t="shared" si="15"/>
         <v>3931</v>
       </c>
-      <c r="AD20">
-        <f t="shared" si="16"/>
+      <c r="AE20">
+        <f t="shared" si="17"/>
         <v>23000</v>
       </c>
-      <c r="AE20">
-        <v>0</v>
-      </c>
       <c r="AF20">
-        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG20">
+        <f t="shared" si="6"/>
         <v>2203</v>
       </c>
     </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>31</v>
       </c>
@@ -2722,11 +2828,11 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <f t="shared" ref="H21:H27" si="17">W21+(65-U21)</f>
+        <f t="shared" ref="H21:H27" si="18">X21+(65-V21)</f>
         <v>2053</v>
       </c>
       <c r="I21">
-        <f>(N21=FALSE)*40+(N21=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J21" t="b">
@@ -2751,67 +2857,70 @@
         <v>0</v>
       </c>
       <c r="P21">
-        <f t="shared" ref="P21:P30" si="18">0.1*$D21</f>
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" ref="Q21:Q30" si="19">0.1*$D21</f>
         <v>100</v>
       </c>
-      <c r="Q21">
-        <f t="shared" ref="Q21:Q25" si="19">0.02*D21</f>
+      <c r="R21">
+        <f t="shared" ref="R21:R25" si="20">0.02*D21</f>
         <v>20</v>
       </c>
-      <c r="R21">
-        <f t="shared" ref="R21:R25" si="20">0.08*D21</f>
+      <c r="S21">
+        <f t="shared" ref="S21:S25" si="21">0.08*D21</f>
         <v>80</v>
       </c>
-      <c r="S21">
-        <f t="shared" ref="S21:S25" si="21">0.015*D21</f>
+      <c r="T21">
+        <f t="shared" ref="T21:T25" si="22">0.015*D21</f>
         <v>15</v>
       </c>
-      <c r="T21" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U21">
+      <c r="U21" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="V21">
         <v>30</v>
       </c>
-      <c r="V21">
-        <v>0</v>
-      </c>
       <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
         <v>2018</v>
       </c>
-      <c r="X21" s="2">
-        <f>MAX(AD21-AC21-36,0)</f>
+      <c r="Y21" s="2">
+        <f>MAX(AE21-AD21-36,0)</f>
         <v>8759</v>
       </c>
-      <c r="Y21" s="2">
-        <f>X21-AE21</f>
+      <c r="Z21" s="2">
+        <f>Y21-AF21</f>
         <v>8759</v>
       </c>
-      <c r="Z21" s="1">
-        <f>X21+MAX(F21*12-801,0)</f>
+      <c r="AA21" s="1">
+        <f>Y21+MAX(F21*12-801,0)</f>
         <v>8759</v>
       </c>
-      <c r="AA21" s="1">
-        <f>MAX(Z21-AE21,0)</f>
+      <c r="AB21" s="1">
+        <f>MAX(AA21-AF21,0)</f>
         <v>8759</v>
       </c>
-      <c r="AC21">
-        <f t="shared" si="14"/>
+      <c r="AD21">
+        <f t="shared" si="15"/>
         <v>2205</v>
       </c>
-      <c r="AD21">
-        <f t="shared" si="16"/>
+      <c r="AE21">
+        <f t="shared" si="17"/>
         <v>11000</v>
       </c>
-      <c r="AE21">
-        <v>0</v>
-      </c>
       <c r="AF21">
-        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG21">
+        <f t="shared" si="6"/>
         <v>1341</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>32</v>
       </c>
@@ -2834,11 +2943,11 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2053</v>
       </c>
       <c r="I22">
-        <f>(N22=FALSE)*40+(N22=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J22" t="b">
@@ -2863,68 +2972,71 @@
         <v>0</v>
       </c>
       <c r="P22">
-        <f t="shared" si="18"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="Q22">
         <f t="shared" si="19"/>
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="R22">
         <f t="shared" si="20"/>
-        <v>240</v>
+        <v>60</v>
       </c>
       <c r="S22">
         <f t="shared" si="21"/>
+        <v>240</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="22"/>
         <v>45</v>
       </c>
-      <c r="T22" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U22">
+      <c r="U22" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="V22">
         <v>30</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>2</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>2018</v>
       </c>
-      <c r="X22" s="2">
-        <f>0.5*(AD22+AD23-(AC22+AC23)-2*36)</f>
+      <c r="Y22" s="2">
+        <f>0.5*(AE22+AE23-(AD22+AD23)-2*36)</f>
         <v>24050.5</v>
       </c>
-      <c r="Y22" s="2">
-        <f>X22-AE22</f>
+      <c r="Z22" s="2">
+        <f>Y22-AF22</f>
         <v>16622.5</v>
       </c>
-      <c r="Z22" s="1">
-        <f>X22+MAX(0.5*(F22*12-(2*801)),0)</f>
+      <c r="AA22" s="1">
+        <f>Y22+MAX(0.5*(F22*12-(2*801)),0)</f>
         <v>24449.5</v>
       </c>
-      <c r="AA22" s="1">
-        <f>MAX(Z22-AE22,0)</f>
+      <c r="AB22" s="1">
+        <f>MAX(AA22-AF22,0)</f>
         <v>17021.5</v>
       </c>
-      <c r="AC22">
-        <f t="shared" si="14"/>
+      <c r="AD22">
+        <f t="shared" si="15"/>
         <v>5896</v>
       </c>
-      <c r="AD22">
-        <f t="shared" si="16"/>
+      <c r="AE22">
+        <f t="shared" si="17"/>
         <v>35000</v>
       </c>
-      <c r="AE22">
+      <c r="AF22">
         <f>7428/2*2</f>
         <v>7428</v>
       </c>
-      <c r="AF22">
-        <f t="shared" si="5"/>
+      <c r="AG22">
+        <f t="shared" si="6"/>
         <v>3304</v>
       </c>
     </row>
-    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>32</v>
       </c>
@@ -2947,11 +3059,11 @@
         <v>0</v>
       </c>
       <c r="H23">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2053</v>
       </c>
       <c r="I23">
-        <f>(N23=FALSE)*40+(N23=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J23" t="b">
@@ -2976,68 +3088,71 @@
         <v>0</v>
       </c>
       <c r="P23">
-        <f t="shared" si="18"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="Q23">
         <f t="shared" si="19"/>
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="R23">
         <f t="shared" si="20"/>
-        <v>160</v>
+        <v>40</v>
       </c>
       <c r="S23">
         <f t="shared" si="21"/>
+        <v>160</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="22"/>
         <v>30</v>
       </c>
-      <c r="T23" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U23">
+      <c r="U23" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="V23">
         <v>30</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>2</v>
       </c>
-      <c r="W23">
+      <c r="X23">
         <v>2018</v>
       </c>
-      <c r="X23" s="2">
-        <f>0.5*(AD22+AD23-(AC22+AC23)-2*36)</f>
+      <c r="Y23" s="2">
+        <f>0.5*(AE22+AE23-(AD22+AD23)-2*36)</f>
         <v>24050.5</v>
       </c>
-      <c r="Y23" s="2">
-        <f>X23-AE23</f>
+      <c r="Z23" s="2">
+        <f>Y23-AF23</f>
         <v>16622.5</v>
       </c>
-      <c r="Z23" s="1">
-        <f>X22+MAX(0.5*(F22*12-(2*801)),0)</f>
+      <c r="AA23" s="1">
+        <f>Y22+MAX(0.5*(F22*12-(2*801)),0)</f>
         <v>24449.5</v>
       </c>
-      <c r="AA23" s="1">
-        <f>MAX(Z23-AE23,0)</f>
+      <c r="AB23" s="1">
+        <f>MAX(AA23-AF23,0)</f>
         <v>17021.5</v>
       </c>
-      <c r="AC23">
-        <f t="shared" si="14"/>
+      <c r="AD23">
+        <f t="shared" si="15"/>
         <v>3931</v>
       </c>
-      <c r="AD23">
-        <f t="shared" si="16"/>
+      <c r="AE23">
+        <f t="shared" si="17"/>
         <v>23000</v>
       </c>
-      <c r="AE23">
+      <c r="AF23">
         <f>7428/2*2</f>
         <v>7428</v>
       </c>
-      <c r="AF23">
-        <f t="shared" si="5"/>
+      <c r="AG23">
+        <f t="shared" si="6"/>
         <v>2203</v>
       </c>
     </row>
-    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>32</v>
       </c>
@@ -3060,11 +3175,11 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2075</v>
       </c>
       <c r="I24">
-        <f>(N24=FALSE)*40+(N24=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J24" t="b">
@@ -3089,7 +3204,6 @@
         <v>0</v>
       </c>
       <c r="P24">
-        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q24">
@@ -3104,40 +3218,44 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="T24" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U24">
+      <c r="T24">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U24" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="V24">
         <v>8</v>
       </c>
-      <c r="V24">
+      <c r="W24">
         <v>2</v>
       </c>
-      <c r="W24">
+      <c r="X24">
         <v>2018</v>
       </c>
-      <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
-      <c r="Z24" s="1"/>
+      <c r="Z24" s="2"/>
       <c r="AA24" s="1"/>
-      <c r="AC24">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
+      <c r="AB24" s="1"/>
       <c r="AD24">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AE24">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AF24">
-        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG24">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>32</v>
       </c>
@@ -3160,11 +3278,11 @@
         <v>0</v>
       </c>
       <c r="H25">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2080</v>
       </c>
       <c r="I25">
-        <f>(N25=FALSE)*40+(N25=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J25" t="b">
@@ -3189,7 +3307,6 @@
         <v>0</v>
       </c>
       <c r="P25">
-        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q25">
@@ -3204,40 +3321,44 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="T25" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U25">
+      <c r="T25">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="U25" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="V25">
         <v>3</v>
       </c>
-      <c r="V25">
+      <c r="W25">
         <v>2</v>
       </c>
-      <c r="W25">
+      <c r="X25">
         <v>2018</v>
       </c>
-      <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
-      <c r="Z25" s="1"/>
+      <c r="Z25" s="2"/>
       <c r="AA25" s="1"/>
-      <c r="AC25">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
+      <c r="AB25" s="1"/>
       <c r="AD25">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AE25">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AF25">
-        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG25">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>33</v>
       </c>
@@ -3260,11 +3381,11 @@
         <v>0</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2043</v>
       </c>
       <c r="I26">
-        <f>(N26=FALSE)*40+(N26=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J26" t="b">
@@ -3285,86 +3406,89 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="O26" s="3">
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26" s="3">
         <v>50</v>
       </c>
-      <c r="P26" s="3">
+      <c r="Q26" s="3">
         <f>0.093*5800</f>
         <v>539.4</v>
       </c>
-      <c r="Q26" s="3">
-        <f t="shared" ref="Q26:Q30" si="22">0.02*D26</f>
+      <c r="R26" s="3">
+        <f t="shared" ref="R26:R30" si="23">0.02*D26</f>
         <v>140</v>
       </c>
-      <c r="R26" s="3">
-        <f t="shared" ref="R26:R30" si="23">0.08*D26</f>
+      <c r="S26" s="3">
+        <f t="shared" ref="S26:S30" si="24">0.08*D26</f>
         <v>560</v>
       </c>
-      <c r="S26" s="3">
-        <f t="shared" ref="S26:S30" si="24">0.015*D26</f>
+      <c r="T26" s="3">
+        <f t="shared" ref="T26:T30" si="25">0.015*D26</f>
         <v>105</v>
       </c>
-      <c r="T26" s="3" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U26" s="3">
-        <v>40</v>
+      <c r="U26" s="3" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="V26" s="3">
+        <v>40</v>
+      </c>
+      <c r="W26" s="3">
         <v>3</v>
       </c>
-      <c r="W26" s="3">
+      <c r="X26" s="3">
         <v>2018</v>
       </c>
-      <c r="X26" s="4">
-        <f>(AG26+AG27)/2</f>
-        <v>38436</v>
-      </c>
       <c r="Y26" s="4">
-        <f>($AJ$26+$AJ$27)/2</f>
-        <v>27294</v>
-      </c>
-      <c r="Z26" s="5">
-        <f>X26+MAX(F26*12-2*801,0)</f>
-        <v>39834</v>
-      </c>
-      <c r="AA26" s="4">
+        <f>(AH26+AH27)/2</f>
+        <v>36738.666666666672</v>
+      </c>
+      <c r="Z26" s="4">
+        <f>($AK$26+$AK$27)/2</f>
+        <v>25596.666666666672</v>
+      </c>
+      <c r="AA26" s="5">
         <f>Y26+MAX(F26*12-2*801,0)</f>
-        <v>28692</v>
-      </c>
-      <c r="AB26" s="3"/>
-      <c r="AC26" s="3">
-        <f t="shared" si="14"/>
+        <v>38136.666666666672</v>
+      </c>
+      <c r="AB26" s="4">
+        <f>Z26+MAX(F26*12-2*801,0)</f>
+        <v>26994.666666666672</v>
+      </c>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3">
+        <f t="shared" si="15"/>
         <v>12371</v>
       </c>
-      <c r="AD26" s="3">
-        <f t="shared" si="16"/>
+      <c r="AE26" s="3">
+        <f t="shared" si="17"/>
         <v>83000</v>
       </c>
-      <c r="AE26">
+      <c r="AF26">
         <f>7428/2*3</f>
         <v>11142</v>
       </c>
-      <c r="AF26" s="3">
-        <f t="shared" si="5"/>
+      <c r="AG26" s="3">
+        <f t="shared" si="6"/>
         <v>7711</v>
       </c>
-      <c r="AG26">
-        <f>AD26-AC26-36-570</f>
-        <v>70023</v>
-      </c>
       <c r="AH26">
-        <f>AG26-AG27</f>
-        <v>63174</v>
-      </c>
-      <c r="AJ26">
-        <f>AG26-(AE26-AI27)</f>
-        <v>54588</v>
-      </c>
-      <c r="AL26" s="3"/>
+        <f>AE26-AD26-(2/3 * 12 * 0.5 *(MIN(4000/12,$O$28)+$O$29))-570</f>
+        <v>68325.666666666672</v>
+      </c>
+      <c r="AI26">
+        <f>AH26-AH27</f>
+        <v>63174.000000000007</v>
+      </c>
+      <c r="AK26">
+        <f>AH26-(AF26-AJ27)</f>
+        <v>51193.333333333343</v>
+      </c>
+      <c r="AM26" s="3"/>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>33</v>
       </c>
@@ -3387,11 +3511,11 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2043</v>
       </c>
       <c r="I27">
-        <f>(N27=FALSE)*40+(N27=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="J27" t="b">
@@ -3416,80 +3540,84 @@
         <v>0</v>
       </c>
       <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
         <f>0.093*$D27</f>
         <v>74.400000000000006</v>
       </c>
-      <c r="Q27">
-        <f t="shared" si="22"/>
-        <v>16</v>
-      </c>
       <c r="R27">
         <f t="shared" si="23"/>
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="S27">
         <f t="shared" si="24"/>
+        <v>64</v>
+      </c>
+      <c r="T27">
+        <f t="shared" si="25"/>
         <v>12</v>
       </c>
-      <c r="T27" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U27">
-        <v>40</v>
+      <c r="U27" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="V27">
+        <v>40</v>
+      </c>
+      <c r="W27">
         <v>3</v>
       </c>
-      <c r="W27">
+      <c r="X27">
         <v>2018</v>
       </c>
-      <c r="X27" s="4">
-        <f>(AG27+AG26)/2</f>
-        <v>38436</v>
-      </c>
       <c r="Y27" s="4">
-        <f>($AJ$26+$AJ$27)/2</f>
-        <v>27294</v>
-      </c>
-      <c r="Z27" s="1">
-        <f>X27+MAX(F27*12-2*801,0)</f>
-        <v>39834</v>
-      </c>
-      <c r="AA27" s="4">
-        <f>Y27+MAX(F26*12-2*801,0)</f>
-        <v>28692</v>
-      </c>
-      <c r="AC27">
-        <f t="shared" si="14"/>
+        <f>(AH27+AH26)/2</f>
+        <v>36738.666666666672</v>
+      </c>
+      <c r="Z27" s="4">
+        <f>($AK$26+$AK$27)/2</f>
+        <v>25596.666666666672</v>
+      </c>
+      <c r="AA27" s="1">
+        <f>Y27+MAX(F27*12-2*801,0)</f>
+        <v>38136.666666666672</v>
+      </c>
+      <c r="AB27" s="4">
+        <f>Z27+MAX(F26*12-2*801,0)</f>
+        <v>26994.666666666672</v>
+      </c>
+      <c r="AD27">
+        <f t="shared" si="15"/>
         <v>1715</v>
       </c>
-      <c r="AD27">
-        <f t="shared" si="16"/>
+      <c r="AE27">
+        <f t="shared" si="17"/>
         <v>8600</v>
       </c>
-      <c r="AE27">
+      <c r="AF27">
         <f>7428/2*3</f>
         <v>11142</v>
       </c>
-      <c r="AF27">
-        <f t="shared" si="5"/>
+      <c r="AG27">
+        <f t="shared" si="6"/>
         <v>1073</v>
       </c>
-      <c r="AG27">
-        <f>AD27-AC27-36</f>
-        <v>6849</v>
-      </c>
-      <c r="AI27">
-        <f>AG27-AE27</f>
-        <v>-4293</v>
+      <c r="AH27">
+        <f>AE27-AD27-(2/3 * 12 * 0.5 *(MIN(4000/12,$O$28)+$O$29))</f>
+        <v>5151.666666666667</v>
       </c>
       <c r="AJ27">
-        <f>AG27-(AE27+AI27)</f>
-        <v>0</v>
-      </c>
+        <f>AH27-AF27</f>
+        <v>-5990.333333333333</v>
+      </c>
+      <c r="AK27">
+        <f>AH27-(AF27+AJ27)</f>
+        <v>0</v>
+      </c>
+      <c r="AM27" s="3"/>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>33</v>
       </c>
@@ -3512,11 +3640,11 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <f t="shared" ref="H28:H30" si="25">W28+(65-U28)</f>
-        <v>2068</v>
+        <f t="shared" ref="H28:H30" si="26">X28+(65-V28)</f>
+        <v>2070</v>
       </c>
       <c r="I28">
-        <f>(N28=FALSE)*40+(N28=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J28" t="b">
@@ -3538,14 +3666,13 @@
         <v>1</v>
       </c>
       <c r="O28">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="P28">
-        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="R28">
@@ -3556,43 +3683,47 @@
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="T28" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U28">
-        <v>15</v>
+      <c r="T28">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="U28" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
       <c r="V28">
+        <v>13</v>
+      </c>
+      <c r="W28">
         <v>3</v>
       </c>
-      <c r="W28">
+      <c r="X28">
         <v>2018</v>
       </c>
-      <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
-      <c r="AC28">
-        <f t="shared" ref="AC28:AC30" si="26">(12*D28+(12*B28 - 1000)*(B28&gt;450))</f>
-        <v>0</v>
-      </c>
+      <c r="AC28" s="1"/>
       <c r="AD28">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="AD28:AD30" si="27">(12*D28+(12*B28 - 1000)*(B28&gt;450))</f>
         <v>0</v>
       </c>
       <c r="AE28">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AF28">
-        <f t="shared" ref="AF28:AF30" si="27">INT(MAX(12 *(0.96*R28+S28), MIN(12 *(0.96*R28+S28+Q28),  1900)  ))</f>
         <v>0</v>
       </c>
       <c r="AG28">
+        <f t="shared" ref="AG28:AG30" si="28">INT(MAX(12 *(0.96*S28+T28), MIN(12 *(0.96*S28+T28+R28),  1900)  ))</f>
+        <v>0</v>
+      </c>
+      <c r="AH28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>33</v>
       </c>
@@ -3615,11 +3746,11 @@
         <v>0</v>
       </c>
       <c r="H29">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2073</v>
       </c>
       <c r="I29">
-        <f>(N29=FALSE)*40+(N29=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J29" t="b">
@@ -3641,14 +3772,13 @@
         <v>1</v>
       </c>
       <c r="O29">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="P29">
-        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="R29">
@@ -3659,43 +3789,47 @@
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="T29" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U29">
+      <c r="T29">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="U29" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="V29">
         <v>10</v>
       </c>
-      <c r="V29">
+      <c r="W29">
         <v>3</v>
       </c>
-      <c r="W29">
+      <c r="X29">
         <v>2018</v>
       </c>
-      <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
       <c r="AB29" s="1"/>
-      <c r="AC29">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
+      <c r="AC29" s="1"/>
       <c r="AD29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AE29">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AF29">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AG29">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AH29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>33</v>
       </c>
@@ -3718,11 +3852,11 @@
         <v>0</v>
       </c>
       <c r="H30">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2075</v>
       </c>
       <c r="I30">
-        <f>(N30=FALSE)*40+(N30=TRUE)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J30" t="b">
@@ -3746,11 +3880,10 @@
         <v>0</v>
       </c>
       <c r="P30">
-        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="22"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="R30">
@@ -3761,39 +3894,43 @@
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="T30" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="U30">
+      <c r="T30">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="U30" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="V30">
         <v>8</v>
       </c>
-      <c r="V30">
+      <c r="W30">
         <v>3</v>
       </c>
-      <c r="W30">
+      <c r="X30">
         <v>2018</v>
       </c>
-      <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
-      <c r="AC30">
-        <f t="shared" si="26"/>
-        <v>0</v>
-      </c>
+      <c r="AC30" s="1"/>
       <c r="AD30">
-        <f t="shared" si="16"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AE30">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="AF30">
-        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AG30">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AH30">
         <v>0</v>
       </c>
     </row>

</xml_diff>